<commit_message>
pull data directly from Google Drive, check new data
</commit_message>
<xml_diff>
--- a/data/raw_data/ManyPrimates_mp1_datasheet_Duke.xlsx
+++ b/data/raw_data/ManyPrimates_mp1_datasheet_Duke.xlsx
@@ -7,11 +7,12 @@
     <sheet state="visible" name="Data" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="1" name="Z_EAAAF3E9_88DC_468B_9EAA_287B5D50E14C_.wvu.FilterData">Data!$A$1:$AD$1159</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Data!$A$1:$AD$955</definedName>
+    <definedName hidden="1" localSheetId="1" name="Z_25FF4D60_993E_476E_AB7E_92893E998F69_.wvu.FilterData">Data!$A$1:$AD$1159</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" tabRatio="600" windowHeight="0" windowWidth="0" guid="{EAAAF3E9-88DC-468B-9EAA-287B5D50E14C}" name="Filter 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" tabRatio="600" windowHeight="0" windowWidth="0" guid="{25FF4D60-993E-476E-AB7E-92893E998F69}" name="Filter 1"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -29834,6 +29835,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
+    <col customWidth="1" min="3" max="3" width="28.86"/>
     <col customWidth="1" min="5" max="5" width="8.86"/>
     <col customWidth="1" min="8" max="8" width="13.0"/>
     <col customWidth="1" min="10" max="12" width="10.0"/>
@@ -80828,8 +80830,9 @@
       <c r="P1159" s="16"/>
     </row>
   </sheetData>
+  <autoFilter ref="$A$1:$AD$955"/>
   <customSheetViews>
-    <customSheetView guid="{EAAAF3E9-88DC-468B-9EAA-287B5D50E14C}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{25FF4D60-993E-476E-AB7E-92893E998F69}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$AD$1159"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
resolve some questions around missing data, add session/block/trial number checks
</commit_message>
<xml_diff>
--- a/data/raw_data/ManyPrimates_mp1_datasheet_Duke.xlsx
+++ b/data/raw_data/ManyPrimates_mp1_datasheet_Duke.xlsx
@@ -8,11 +8,11 @@
   </sheets>
   <definedNames>
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Data!$A$1:$AD$955</definedName>
-    <definedName hidden="1" localSheetId="1" name="Z_25FF4D60_993E_476E_AB7E_92893E998F69_.wvu.FilterData">Data!$A$1:$AD$1159</definedName>
+    <definedName hidden="1" localSheetId="1" name="Z_BF946D28_9660_411F_A4AA_EFFB48DFE915_.wvu.FilterData">Data!$A$1:$AD$1159</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" tabRatio="600" windowHeight="0" windowWidth="0" guid="{25FF4D60-993E-476E-AB7E-92893E998F69}" name="Filter 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" tabRatio="600" windowHeight="0" windowWidth="0" guid="{BF946D28-9660-411F-A4AA-EFFB48DFE915}" name="Filter 1"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -80832,7 +80832,7 @@
   </sheetData>
   <autoFilter ref="$A$1:$AD$955"/>
   <customSheetViews>
-    <customSheetView guid="{25FF4D60-993E-476E-AB7E-92893E998F69}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{BF946D28-9660-411F-A4AA-EFFB48DFE915}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$AD$1159"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
updated vienna & species datasheets
</commit_message>
<xml_diff>
--- a/data/raw_data/ManyPrimates_mp1_datasheet_Duke.xlsx
+++ b/data/raw_data/ManyPrimates_mp1_datasheet_Duke.xlsx
@@ -8,11 +8,11 @@
   </sheets>
   <definedNames>
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Data!$A$1:$AD$1159</definedName>
-    <definedName hidden="1" localSheetId="1" name="Z_2F70E2AC_0C3D_475A_B821_B73DBA6C703F_.wvu.FilterData">Data!$A$1:$AD$1159</definedName>
+    <definedName hidden="1" localSheetId="1" name="Z_61D06A49_A8DB_4021_908C_FE9507F872B1_.wvu.FilterData">Data!$A$1:$AD$1159</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" tabRatio="600" windowHeight="0" windowWidth="0" guid="{2F70E2AC-0C3D-475A-B821-B73DBA6C703F}" name="Filter 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" tabRatio="600" windowHeight="0" windowWidth="0" guid="{61D06A49-A8DB-4021-908C-FE9507F872B1}" name="Filter 1"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -82767,7 +82767,7 @@
   </sheetData>
   <autoFilter ref="$A$1:$AD$1159"/>
   <customSheetViews>
-    <customSheetView guid="{2F70E2AC-0C3D-475A-B821-B73DBA6C703F}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{61D06A49-A8DB-4021-908C-FE9507F872B1}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$AD$1159"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>